<commit_message>
MovingSum compared to MovingAverage. TODO get python sheets automation to receive testing range as parameter
</commit_message>
<xml_diff>
--- a/GeneticProgrammingPortfolio/experiment-data/1 - math/with iflt/23-00-27/data.xlsx
+++ b/GeneticProgrammingPortfolio/experiment-data/1 - math/with iflt/23-00-27/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\GPP\GeneticProgrammingPortfolio\experiment-data\exp-1\with iflt\23-00-27\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\GPP\GeneticProgrammingPortfolio\experiment-data\1 - math\with iflt\23-00-27\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Math, with IFLT" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="1" r:id="rId2"/>
+    <sheet name="Chart1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1785,7 +1786,1667 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DJIA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$A$2:$A$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.84026811000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83498734399999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85444194600000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86634980399999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86080725199999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83614498199999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84682125600000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83154587999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82724681099999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.820568721</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83020295200000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.80361808499999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.80763326899999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.82765563900000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.82657704700000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.84360672999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.86945043700000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.87061997400000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.88099791400000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.89276637999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.89563412499999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.89966035799999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.89541313700000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.88205695699999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.90050096300000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.90680932299999994</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.90804770599999995</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.90690621800000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.90278393999999995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.93002922099999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.94341940000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.94140925799999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93787174900000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.95470849099999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.95269239999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.94485072299999995</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.95889366600000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.96649140600000005</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.96219318799999998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.96184045699999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.96582674199999996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.950540316</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.95289723900000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.94813834500000005</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.92653675999999996</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.90929713899999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.92950650000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.93005811999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.95110808499999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.95073325500000005</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.958472938</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.95582703099999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.95748529199999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.95758728599999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.956320854</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.94964276400000003</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.96395854299999995</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.95047232000000004</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.92905262399999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.96049752899999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.95054286600000004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.93673026000000004</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.93029610699999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.93730397899999995</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.91099449700000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.91977367399999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.933067808</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.95212208099999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.93059699100000004</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.89937902300000006</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.90983941000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.92391890099999996</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.93967195199999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.93538478300000005</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.933353392</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.94973285900000004</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.93977904599999995</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.92457846499999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1598-451F-AF42-581163FB2424}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ENS_AVG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$B$2:$B$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.92331621217424331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92273750533118382</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92213745916064505</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9214917192556219</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92081745758972722</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9200803290120193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91929738847078468</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91844057314955496</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91755140457305506</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91658537061231093</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.91556790598465332</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.91444374683449103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91324574175934958</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91199633158407278</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.91055572692629883</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.90905291744548633</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.90745495558426592</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.90573718444537066</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.90382963053293119</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.90170330575667601</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.90907325405068728</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.91527240196673143</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91964983214514417</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.92278396523306006</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.92503281619038169</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.92668422034292908</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.92790044056073762</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.92883741921802798</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.92955599890470386</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.93013661301700601</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.93058612616463476</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.93095837035331452</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93532386048393734</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.93563349832491505</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9358717754486382</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.93612653426307602</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.93627645322263875</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.93644537203290412</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.9366131974188211</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.93673897142798801</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.93687609393807847</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.93699462201654293</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9371387111102365</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.93771963547728931</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.93738020774617148</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.93748474464465714</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.93760320001149566</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.93771488717916662</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.93784313056399116</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.93795580496911057</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.93807387496996875</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.94063584562636204</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.94066407598398027</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.94072908027179458</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.94077668688751437</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.94086565757988772</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.94097260808031724</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.9411432471574166</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.94119722298009045</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.94131920579755279</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.94139917106106696</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.94157971941141805</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.94170961920531915</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.94184859574845259</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.94196987040938607</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.94210760994037113</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.94224021120408985</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.94239176133130742</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.94252985209218809</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.94267326077877167</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.94280250314812486</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.94294965762037186</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.94309142998301076</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.94324750851311134</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.94338751405589516</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.94353393045676437</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.94364886371924983</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.94381998027905123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1598-451F-AF42-581163FB2424}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ENS_MED</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$C$2:$C$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.9315075980855666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93148823528785407</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93146731523028503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93144486478590149</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93142092730347692</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93139556342603502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93136885410431081</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93134090244859546</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9313118317265201</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93128177992537986</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.93125089400510974</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93121932682134334</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93118723687586447</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9311547881711657</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.93112214714756636</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9310894762199996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93105692646947313</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.93102463281084702</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.93099271278091433</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.93096126698518344</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.93093037804605139</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.93090010667063972</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.93087048654065174</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.93084152127902842</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.93081318535424074</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.93078542772960171</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.93075817513888282</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.93073133279945508</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.93070478326599881</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.93067838630972088</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.93065198218615275</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.93062539792464982</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93146075831023789</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.93141763103829289</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.93137391405281234</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.93132951748540371</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.93128435285175504</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.93123833611662743</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.93151714173294664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.93202908264495243</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.93245057176046853</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.93279800563779769</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9330843821585818</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.93498775513899679</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.93351346033295368</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.93367128145888889</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.93379906671153845</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.93390134975202788</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.93398187860502824</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.93404377224700486</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.93408964331217548</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.93711017722687595</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.93721701608002239</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.937303524483866</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.93737244932420061</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.93742617060930122</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.93746676512331339</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.93749605804908609</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.93751566497130112</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.93752702614668226</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.93753143452588239</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.93753005870138661</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.93752396171524222</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.93751411647308158</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.93750141836435419</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.93748669557355924</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.93747071747648847</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.93745420144363345</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.93747155212269695</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.93789738598900729</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.93832764137398716</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.9387621877050325</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.93920089493134118</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.93964363359453795</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.94009027489836205</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.94054069077734515</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.94099475396443477</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.94145233805748862</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1598-451F-AF42-581163FB2424}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ENS_MIN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$D$2:$D$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.85327853243416119</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85321910191239991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85315934958045636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85309927703077215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85303888584808818</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85297817760949168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85291715388446343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85285581623492346</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.85279416621527793</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.85273220537246441</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.85266993524599766</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85260735736801463</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.85254447326331939</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.85248128444942761</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85241779243661076</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.85235399872794027</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.85228990481933076</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85222551219958365</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.85216082235043</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8520958367465733</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.85203055685573181</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.85196498413868071</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.8518991200492938</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.85183296603458525</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.85176652353475069</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.85169979398320794</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.85755193320412415</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.85755191794408647</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.85755189701678436</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.85755187917989284</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.8575518561061477</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.85755184296756981</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.91734481083538666</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.91826107960063186</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9183360784207879</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.91841090101917366</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.91848554826965489</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.91856002103931444</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.91863432018851554</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9187084465709634</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.91878240103376707</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.91885618441750128</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.91892979755626603</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.88503198070811551</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.91907651640327803</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.91914962374789411</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.91922256412039649</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.91929533832340726</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.91936794715342829</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.91944039140089784</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.91951267185024776</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.89161778952501869</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.89258903553609503</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.89359165155551235</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.89462510640585091</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.89568884255328141</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.89678227640881103</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.89790479864907735</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.89905577455654495</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.90023454437896056</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.90144042370793842</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.90267270387651499</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.90393065237550496</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.90521351328848942</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.90652050774524395</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.90785083439342074</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.90920366988825652</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.91057816940009995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.91197346713951943</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.91338867689972847</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.91482289261609229</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.91627518894240445</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.917744621843682</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.91917089551107434</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.91904042297725863</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.9189106188996603</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.91878148496470113</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.91865302277381156</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1598-451F-AF42-581163FB2424}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ENS_MAX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$E$2:$E$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>0.97826074608608937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97833057735253026</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97869161139116356</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97893699338834961</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97947105434791837</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97970866775421783</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98003359851769234</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9799978939293833</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98049506920983409</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98077637191129874</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98142288824955526</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98151051027148362</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.981812879540646</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98290252685603408</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98227647949373809</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98257958224701603</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98220665656121098</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98330568486941472</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98358908208094398</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.98399097107248579</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98403503656579383</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.98436408503462181</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.98456047310811523</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.98510317422157734</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.9853590258644509</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98569230335716829</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.98574086222401702</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.98612889325901254</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.98638718184938545</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98692684474026748</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9871176502258453</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98742294112009654</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.986998529605015</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.98787484316549135</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.98815951937184199</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.98925580828824511</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.98887052912764406</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.98915695952580862</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.98966471693097646</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.98960262437667301</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.98990843762075442</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.98999403567387134</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.99061952917378471</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.9908842511012681</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.99123497192752352</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.99129609686730202</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.9916358003425817</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.99186347830623145</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.99237426330221634</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9926018926439848</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.99291222285006142</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.99288919636168615</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.99334705973052828</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.99361257136143977</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.99421444226919498</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.99431412703298283</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.99460279593910794</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.99597225367398956</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.99504115112955005</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.99532758386383124</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.99473975401493031</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.99601846215358825</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.99628789722194955</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.99667863262379963</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.99670910567840765</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.99701958794983092</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.99719653148212273</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.9977219529002781</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.99796635876395889</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.9982861218215684</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.99833218650915967</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.99869669096050073</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.99893952688746834</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.99945249496427691</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.99963864255477131</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.999930111285527</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.99962110582949459</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.0003559254020331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1598-451F-AF42-581163FB2424}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="401748440"/>
+        <c:axId val="402832384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="401748440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402832384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="402832384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401748440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2341,6 +4002,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -2352,11 +4529,49 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8665679" cy="6284429"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2666,8 +4881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>